<commit_message>
Change in Excel Spreadsheet
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>I was changed in NewBranch1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,15 +358,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -366,7 +374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+B1</f>
         <v>3</v>
@@ -374,6 +382,14 @@
       <c r="B2">
         <f>SUM(A1:A2,B1)</f>
         <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>